<commit_message>
Actualizacion de formateos de diversas cosas
</commit_message>
<xml_diff>
--- a/ExcelManager/Plantilla/Plantilla_Factura.xlsx
+++ b/ExcelManager/Plantilla/Plantilla_Factura.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleze\Desktop\PPS\Facturador-Electronico-AFIP-ARCA\ExcelManager\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6793BFC7-ECAE-481E-ADA2-EB7C69B71A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F17CCB-00C2-41B4-817D-34165731D2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="417" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="417" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Facturas_A_Realizar" sheetId="5" r:id="rId1"/>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75414389-46C2-464F-B457-CE7D8944C46B}">
   <dimension ref="A1:N101"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5703125" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2195,15 +2195,6 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G101" xr:uid="{6E558A0D-88A1-4D2B-8E57-0B364EC784BE}">
-      <formula1>"Consumidor Final"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2:D101" xr:uid="{7382F4FD-EF70-4BD7-97D5-EC0C7E31FF86}">
-      <formula1>"CUIT,DNI,CDI,CI EXTRANJERA,PASAPORTE,OTRO"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F101" xr:uid="{9950C601-4FF5-489A-A73A-4E8E2C730769}">
-      <formula1>"ENTREGA INMEDIATA,CONTADO,CRÉDITO A 30 DÍAS,PAGO ANTICIPADO"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:B101" xr:uid="{A673E2EA-42F7-4E93-9A5E-2193328D7378}">
       <formula1>"Factura C"</formula1>
     </dataValidation>
@@ -2212,6 +2203,15 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H2:H101" xr:uid="{FCBF3425-C5CB-43F2-8871-60B194B637BC}">
       <formula1>"PRODUCTOS,SERVICIOS,PRODUCTOS Y SERVICIOS"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="D2:D1048576" xr:uid="{36050D77-F43B-4438-A4A1-A6D6358119FD}">
+      <formula1>"CONSUMIDOR FINAL, CUIT,DNI,CDI,CI EXTRANJERA,PASAPORTE,"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{2B38F1BF-A1E1-44DC-AC5C-FFB8B122EC17}">
+      <formula1>"Contado,Cuenta Corriente,Tarjeta de Crédito,Tarjeta de Débito,Cheque,Transferencia,Pago Anticipado,Crédito a 30 días"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{A106C764-CAFC-4A58-8E89-BE4BB58DDA6A}">
+      <formula1>"Consumidor Final, Monotributista, Excento"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2463,8 +2463,8 @@
   </sheetPr>
   <dimension ref="A1:XFC500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AM8" sqref="AM8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Configuracion de los Iframes para los videos
</commit_message>
<xml_diff>
--- a/ExcelManager/Plantilla/Plantilla_Factura.xlsx
+++ b/ExcelManager/Plantilla/Plantilla_Factura.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleze\Desktop\PPS\Facturador-Electronico-AFIP-ARCA\ExcelManager\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F17CCB-00C2-41B4-817D-34165731D2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64E9C9E-A99D-40B3-A30D-DACD51CEBF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="417" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="XML" sheetId="6" state="hidden" r:id="rId2"/>
     <sheet name="Datos" sheetId="4" state="hidden" r:id="rId3"/>
     <sheet name="Items" sheetId="2" state="hidden" r:id="rId4"/>
-    <sheet name="Historial" sheetId="3" r:id="rId5"/>
+    <sheet name="Historial" sheetId="3" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="ListaDesplegable">OFFSET(Items!#REF!,0,0,COUNTA(Items!#REF!),1)</definedName>

</xml_diff>

<commit_message>
Actualización IVA Factura A y B
</commit_message>
<xml_diff>
--- a/ExcelManager/Plantilla/Plantilla_Factura.xlsx
+++ b/ExcelManager/Plantilla/Plantilla_Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleze\Desktop\PPS\Facturador-Electronico-AFIP-ARCA\ExcelManager\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046288BC-949F-4805-B428-F9010EFAB9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E578A30-A657-456A-BF3F-D7064F328E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="417" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="417" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Factura_C" sheetId="5" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="68">
   <si>
     <t>Identificador Factura</t>
   </si>
@@ -243,12 +243,21 @@
   <si>
     <t>Nombre Apellido del Cliente</t>
   </si>
+  <si>
+    <t>Base 21%</t>
+  </si>
+  <si>
+    <t>Base 10.5%</t>
+  </si>
+  <si>
+    <t>Base 0%</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -302,6 +311,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -323,7 +338,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -362,11 +377,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -398,6 +428,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6243,8 +6274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF1BF8-01C8-494B-93EA-208B81931AFC}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6531,10 +6562,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:XFC500"/>
+  <dimension ref="A1:XFD500"/>
   <sheetViews>
-    <sheetView topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="AU1" sqref="AU1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+      <selection activeCell="AX1" sqref="AX1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -6582,14 +6613,15 @@
     <col min="41" max="41" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="25" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="25.7109375" customWidth="1"/>
-    <col min="45" max="45" width="15.42578125" style="12" customWidth="1"/>
-    <col min="46" max="46" width="16" style="12" customWidth="1"/>
-    <col min="47" max="16383" width="7.85546875" style="12" hidden="1"/>
-    <col min="16384" max="16384" width="11.5703125" style="12" hidden="1"/>
+    <col min="44" max="45" width="25.7109375" customWidth="1"/>
+    <col min="46" max="46" width="15.42578125" style="12" customWidth="1"/>
+    <col min="47" max="47" width="16" style="12" customWidth="1"/>
+    <col min="48" max="49" width="11.5703125" style="12" customWidth="1"/>
+    <col min="50" max="16383" width="11.5703125" style="12" hidden="1"/>
+    <col min="16384" max="16384" width="16" style="12" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6722,28 +6754,37 @@
       <c r="AR1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AS1" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="AT1" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="AU1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="AV1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AW1" s="14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="4" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Creacion de Obtenedor PDF para mayor claridad
</commit_message>
<xml_diff>
--- a/ExcelManager/Plantilla/Plantilla_Factura.xlsx
+++ b/ExcelManager/Plantilla/Plantilla_Factura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eleze\Desktop\PPS\Facturador-Electronico-AFIP-ARCA\ExcelManager\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E578A30-A657-456A-BF3F-D7064F328E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B8E098C-3D7D-4303-8E3B-0D610B8F54FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="417" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="417" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Factura_C" sheetId="5" r:id="rId1"/>
@@ -2351,7 +2351,7 @@
   <dimension ref="A1:S101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5703125" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4157,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49277A82-554C-46BD-9187-CDB4C7B39064}">
   <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5703125" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -6249,9 +6249,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J1048576" xr:uid="{5876F54E-97E5-416D-84AC-DF138578BBBB}">
       <formula1>"Contado,Cuenta Corriente,Tarjeta de Crédito,Tarjeta de Débito,Cheque,Transferencia,Pago Anticipado,Crédito a 30 días"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C2:C1048576" xr:uid="{FA53A828-681F-4CDB-85EC-FA9481302A5F}">
-      <formula1>"CONSUMIDOR FINAL, CUIT,DNI,CDI,CI EXTRANJERA,PASAPORTE,"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L2:L101" xr:uid="{BCC2D9E0-0909-485A-9503-7F7A7859316F}">
       <formula1>"PRODUCTOS,SERVICIOS,PRODUCTOS Y SERVICIOS"</formula1>
     </dataValidation>
@@ -6263,6 +6260,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{C520E740-DF8F-489D-B001-AE3329DB2C9A}">
       <formula1>"Responsable Inscripto"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C2:C1048576" xr:uid="{FE68CEE6-E8E9-45D7-99B1-3B28BD83AA1B}">
+      <formula1>"CUIT"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6562,9 +6562,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:XFD500"/>
+  <dimension ref="A1:XFC500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+    <sheetView topLeftCell="AQ1" workbookViewId="0">
       <selection activeCell="AX1" sqref="AX1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>